<commit_message>
Start develop MVC5=> MVC6 Tool
</commit_message>
<xml_diff>
--- a/Common/Template/ModelTemplate.xlsx
+++ b/Common/Template/ModelTemplate.xlsx
@@ -692,7 +692,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -765,12 +765,60 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -795,53 +843,11 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1141,17 +1147,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="10" style="1"/>
     <col min="2" max="11" width="13.625" style="1" customWidth="1"/>
-    <col min="12" max="29" width="10" style="1"/>
+    <col min="12" max="26" width="10" style="1"/>
+    <col min="27" max="27" width="13.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="10" style="1"/>
+    <col min="29" max="29" width="14.875" style="1" customWidth="1"/>
     <col min="30" max="30" width="16" style="1" customWidth="1"/>
     <col min="31" max="31" width="18.375" style="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5" style="1" customWidth="1"/>
+    <col min="32" max="32" width="20.25" style="1" customWidth="1"/>
     <col min="33" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
@@ -1162,25 +1171,25 @@
       <c r="B2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
       <c r="K2" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="49">
+      <c r="L2" s="24">
         <v>1</v>
       </c>
-      <c r="M2" s="49"/>
+      <c r="M2" s="24"/>
       <c r="AA2" s="5" t="s">
         <v>53</v>
       </c>
@@ -1196,7 +1205,7 @@
       <c r="AE2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AF2" s="2" t="s">
         <v>60</v>
       </c>
       <c r="AJ2" s="15" t="s">
@@ -1231,28 +1240,28 @@
       <c r="B3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
       <c r="E3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="AA3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AB3" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AC3" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="2"/>
+      <c r="AD3" s="51"/>
       <c r="AJ3" s="19" t="s">
         <v>25</v>
       </c>
@@ -1294,135 +1303,135 @@
       </c>
     </row>
     <row r="5" spans="1:48" ht="18.75" customHeight="1">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="40" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="40"/>
-      <c r="K5" s="40"/>
-      <c r="L5" s="41" t="s">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="41"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="29" t="s">
+      <c r="M5" s="35"/>
+      <c r="N5" s="36"/>
+      <c r="O5" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="30"/>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
-      <c r="U5" s="30"/>
-      <c r="V5" s="30"/>
-      <c r="W5" s="30"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="32" t="s">
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="24" t="s">
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="24"/>
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="41"/>
     </row>
     <row r="6" spans="1:48" ht="14.25" customHeight="1">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="45" t="s">
+      <c r="K6" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="38" t="s">
+      <c r="N6" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="25" t="s">
+      <c r="O6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25" t="s">
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="25"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="26" t="s">
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="27"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="26" t="s">
+      <c r="U6" s="43"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="34" t="s">
+      <c r="X6" s="44"/>
+      <c r="Y6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="Z6" s="34" t="s">
+      <c r="Z6" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="AA6" s="25" t="s">
+      <c r="AA6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="AB6" s="25" t="s">
+      <c r="AB6" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="AC6" s="25" t="s">
+      <c r="AC6" s="34" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:48" ht="14.25" customHeight="1">
-      <c r="B7" s="44"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
       <c r="O7" s="9" t="s">
         <v>17</v>
       </c>
@@ -1453,11 +1462,11 @@
       <c r="X7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="25"/>
-      <c r="AB7" s="25"/>
-      <c r="AC7" s="25"/>
+      <c r="Y7" s="33"/>
+      <c r="Z7" s="33"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="34"/>
+      <c r="AC7" s="34"/>
     </row>
     <row r="8" spans="1:48">
       <c r="B8" s="2"/>
@@ -2481,13 +2490,18 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="AA5:AC5"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="AC6:AC7"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="O5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="Z6:Z7"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="F5:K5"/>
@@ -2504,18 +2518,13 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="I6:I7"/>
-    <mergeCell ref="AA5:AC5"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="AC6:AC7"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="O5:X5"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="4">

</xml_diff>

<commit_message>
增加无特性模式在C#的Entity做成中 CompanyTable -> OwnerTable
</commit_message>
<xml_diff>
--- a/Common/Template/ModelTemplate.xlsx
+++ b/Common/Template/ModelTemplate.xlsx
@@ -52,7 +52,7 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>正则表达</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>布尔值</t>
@@ -68,253 +68,237 @@
   </si>
   <si>
     <t>数据使用类型</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>格式</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>版本控制</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>必须项目</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>数值范围</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>字符串长度</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>模式</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>表示</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>备注</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>更新者</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>更新日期</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>电子邮件</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>是/否</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>错误信息</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>最小值</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>最大值</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>密码</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>日期</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>时间</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>日期时间</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>元数据类型枚举</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>元数据类型</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>普通枚举</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>旗标枚举</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Key项目</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>长度</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>默认值</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>领域专家填写</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>开发人员填写</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>含义</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>输入规则</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>数据库设计</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>用户交互设计</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>领域项目名称</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>变量名称</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>数据模型名称</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>名字空间名称</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>数据集名称</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>主键前缀</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>数据使用类型</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>列表类型</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>继承</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>EntityBase</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>MasterTable</t>
   </si>
   <si>
     <t>说明标题</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>画面表示名称</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>标记</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>HIDDEN</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SuperClass</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Flag</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>SKIP</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>枚举/Master类型</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>辅助表</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>辅助评价表</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>StatusMasterTable</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>CatalogMasterTable</t>
   </si>
   <si>
     <t>手机</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>目录表</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>ompanyTable</t>
-    </r>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>目录类型</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>单精度浮点</t>
@@ -327,14 +311,18 @@
   </si>
   <si>
     <t>版本号</t>
-    <phoneticPr fontId="7" type="noConversion"/>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>OwnerTable</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,13 +330,6 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -696,119 +677,119 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -816,38 +797,38 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,7 +1128,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD11" sqref="AD11"/>
+      <selection pane="topRight" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="16.5"/>
@@ -1171,33 +1152,33 @@
       <c r="B2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
       <c r="K2" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" s="24">
+        <v>67</v>
+      </c>
+      <c r="L2" s="26">
         <v>1</v>
       </c>
-      <c r="M2" s="24"/>
+      <c r="M2" s="26"/>
       <c r="AA2" s="5" t="s">
         <v>53</v>
       </c>
       <c r="AB2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="14" t="s">
-        <v>63</v>
+      <c r="AC2" s="25" t="s">
+        <v>68</v>
       </c>
       <c r="AD2" s="2" t="s">
         <v>48</v>
@@ -1208,230 +1189,230 @@
       <c r="AF2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AJ2" s="15" t="s">
+      <c r="AJ2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AK2" s="16" t="s">
+      <c r="AK2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="16" t="s">
+      <c r="AL2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AM2" s="16" t="s">
+      <c r="AM2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="AN2" s="16" t="s">
+      <c r="AN2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="AO2" s="16" t="s">
+      <c r="AO2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AP2" s="17" t="s">
+      <c r="AP2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="AQ2" s="16"/>
-      <c r="AR2" s="16"/>
-      <c r="AS2" s="16"/>
-      <c r="AT2" s="16"/>
-      <c r="AU2" s="16"/>
-      <c r="AV2" s="18"/>
+      <c r="AQ2" s="15"/>
+      <c r="AR2" s="15"/>
+      <c r="AS2" s="15"/>
+      <c r="AT2" s="15"/>
+      <c r="AU2" s="15"/>
+      <c r="AV2" s="17"/>
     </row>
     <row r="3" spans="1:48" ht="17.25" thickBot="1">
       <c r="B3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
       <c r="AA3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="50" t="s">
+      <c r="AB3" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="AC3" s="51" t="s">
+      <c r="AC3" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="AD3" s="51"/>
-      <c r="AJ3" s="19" t="s">
+      <c r="AD3" s="24"/>
+      <c r="AJ3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="AK3" s="20" t="s">
+      <c r="AK3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="AL3" s="20" t="s">
+      <c r="AL3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AM3" s="20" t="s">
+      <c r="AM3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="AN3" s="20" t="s">
+      <c r="AN3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AO3" s="21" t="s">
+      <c r="AO3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="AP3" s="21" t="s">
+      <c r="AQ3" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="AQ3" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="AR3" s="20" t="s">
+      <c r="AR3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AS3" s="20" t="s">
+      <c r="AS3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="AT3" s="22" t="s">
+      <c r="AT3" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AU3" s="22" t="s">
+      <c r="AU3" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AV3" s="23" t="s">
+      <c r="AV3" s="22" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:48" ht="18.75" customHeight="1">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="31" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="35" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="M5" s="35"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="45" t="s">
+      <c r="M5" s="37"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="47"/>
-      <c r="Y5" s="48" t="s">
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="Z5" s="49"/>
-      <c r="AA5" s="41" t="s">
+      <c r="Z5" s="51"/>
+      <c r="AA5" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="AB5" s="41"/>
-      <c r="AC5" s="41"/>
+      <c r="AB5" s="43"/>
+      <c r="AC5" s="43"/>
     </row>
     <row r="6" spans="1:48" ht="14.25" customHeight="1">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="34" t="s">
+      <c r="G6" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="I6" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="32" t="s">
+      <c r="I6" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="K6" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="29" t="s">
+      <c r="L6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="29" t="s">
+      <c r="M6" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="29" t="s">
+      <c r="N6" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="34" t="s">
+      <c r="O6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="34" t="s">
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="R6" s="34"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="42" t="s">
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="U6" s="43"/>
-      <c r="V6" s="44"/>
-      <c r="W6" s="42" t="s">
+      <c r="U6" s="45"/>
+      <c r="V6" s="46"/>
+      <c r="W6" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="32" t="s">
+      <c r="X6" s="46"/>
+      <c r="Y6" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="Z6" s="32" t="s">
+      <c r="Z6" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="AA6" s="34" t="s">
+      <c r="AA6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AB6" s="34" t="s">
+      <c r="AB6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="AC6" s="34" t="s">
+      <c r="AC6" s="36" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:48" ht="14.25" customHeight="1">
-      <c r="B7" s="38"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
       <c r="O7" s="9" t="s">
         <v>17</v>
       </c>
@@ -1462,11 +1443,11 @@
       <c r="X7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="Y7" s="33"/>
-      <c r="Z7" s="33"/>
-      <c r="AA7" s="34"/>
-      <c r="AB7" s="34"/>
-      <c r="AC7" s="34"/>
+      <c r="Y7" s="35"/>
+      <c r="Z7" s="35"/>
+      <c r="AA7" s="36"/>
+      <c r="AB7" s="36"/>
+      <c r="AC7" s="36"/>
     </row>
     <row r="8" spans="1:48">
       <c r="B8" s="2"/>
@@ -2526,7 +2507,7 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I2:J2"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:J2">
       <formula1>$AB$2:$AF$2</formula1>

</xml_diff>